<commit_message>
Added a new method in formatting.py called renameCSV. It renames the .csv files downloaded through extractHistorical to the name of the respective ticker.
</commit_message>
<xml_diff>
--- a/bin/net_income.xlsx
+++ b/bin/net_income.xlsx
@@ -1,39 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cummi\Desktop\webscrap\bin\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C87A5D-DF96-4E84-AB0D-519725883063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>2022</t>
   </si>
@@ -56,27 +37,35 @@
     <t>pltr</t>
   </si>
   <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>AGR</t>
+    <t>$59,972,000</t>
+  </si>
+  <si>
+    <t>-$373,705</t>
+  </si>
+  <si>
+    <t>$76,033,000</t>
+  </si>
+  <si>
+    <t>-$520,379</t>
+  </si>
+  <si>
+    <t>$40,269,000</t>
+  </si>
+  <si>
+    <t>-$1,166,391</t>
+  </si>
+  <si>
+    <t>$34,343,000</t>
+  </si>
+  <si>
+    <t>-$579,646</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,13 +81,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -108,7 +90,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -131,48 +113,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -219,7 +174,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,27 +206,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,24 +240,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -496,20 +415,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -525,54 +438,40 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
-        <v>59972000</v>
-      </c>
-      <c r="C2" s="2">
-        <v>76033000</v>
-      </c>
-      <c r="D2" s="2">
-        <v>40269000</v>
-      </c>
-      <c r="E2" s="2">
-        <v>34343000</v>
-      </c>
-      <c r="F2" s="3"/>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4">
-        <v>-373705</v>
-      </c>
-      <c r="C3" s="4">
-        <v>-520379</v>
-      </c>
-      <c r="D3" s="4">
-        <v>-1166391</v>
-      </c>
-      <c r="E3" s="4">
-        <v>-579646</v>
-      </c>
-      <c r="F3" s="3"/>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>